<commit_message>
Updated addOnOrder for both retail and personal. Tried test suite collection parallelism.
</commit_message>
<xml_diff>
--- a/NewArrivals/contactData.xlsx
+++ b/NewArrivals/contactData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\TestAutomation\NewArrivals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\testautomation\NewArrivals\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>firstName</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>TAMPA</t>
+  </si>
+  <si>
+    <t>neoguest2</t>
+  </si>
+  <si>
+    <t>neoguest2ab@test.com</t>
+  </si>
+  <si>
+    <t>PLANT CITY</t>
+  </si>
+  <si>
+    <t>1908 INDUSTRIAL PARK DR</t>
   </si>
 </sst>
 </file>
@@ -517,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -624,6 +636,29 @@
         <v>33629</v>
       </c>
     </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>33566</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
@@ -633,9 +668,11 @@
     <hyperlink ref="C3" r:id="rId4"/>
     <hyperlink ref="F4" r:id="rId5" display="C@bi$ush5"/>
     <hyperlink ref="C4" r:id="rId6"/>
+    <hyperlink ref="C5" r:id="rId7"/>
+    <hyperlink ref="F5" r:id="rId8" display="C@bi$ush5"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Fixed issues with Edit Order
</commit_message>
<xml_diff>
--- a/NewArrivals/contactData.xlsx
+++ b/NewArrivals/contactData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\testautomation_new\EditOrder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\testautomation\NewArrivals\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>firstName</t>
   </si>
@@ -57,9 +57,6 @@
     <t>DADE CITY</t>
   </si>
   <si>
-    <t>FLORIDA</t>
-  </si>
-  <si>
     <t>neocohost1</t>
   </si>
   <si>
@@ -111,7 +108,7 @@
     <t>TROY</t>
   </si>
   <si>
-    <t>MICHIGAN</t>
+    <t>Florida</t>
   </si>
 </sst>
 </file>
@@ -565,7 +562,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -616,8 +613,8 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
+      <c r="F2" t="s">
+        <v>29</v>
       </c>
       <c r="G2">
         <v>33523</v>
@@ -625,22 +622,22 @@
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
+      <c r="F3" t="s">
+        <v>29</v>
       </c>
       <c r="G3">
         <v>33166</v>
@@ -648,22 +645,22 @@
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
+      <c r="F4" t="s">
+        <v>29</v>
       </c>
       <c r="G4">
         <v>33629</v>
@@ -671,22 +668,22 @@
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>12</v>
+      <c r="F5" t="s">
+        <v>29</v>
       </c>
       <c r="G5">
         <v>33566</v>
@@ -694,22 +691,22 @@
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
       </c>
       <c r="G6">
         <v>48085</v>
@@ -718,18 +715,14 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="C@bi$ush5"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="F3" r:id="rId3" display="C@bi$ush5"/>
-    <hyperlink ref="C3" r:id="rId4"/>
-    <hyperlink ref="F4" r:id="rId5" display="C@bi$ush5"/>
-    <hyperlink ref="C4" r:id="rId6"/>
-    <hyperlink ref="C5" r:id="rId7"/>
-    <hyperlink ref="F5" r:id="rId8" display="C@bi$ush5"/>
-    <hyperlink ref="C6" r:id="rId9"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>